<commit_message>
Minor Bugfixing Planung A, B, D 18.11.2021
</commit_message>
<xml_diff>
--- a/SCRUM/SCRUM_TEAM_A.xlsx
+++ b/SCRUM/SCRUM_TEAM_A.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>PO - Backlog</t>
   </si>
@@ -113,7 +113,13 @@
     <t>Spezifikation neues Spiel.</t>
   </si>
   <si>
-    <t>Überplant</t>
+    <t>Time-Limit fertig machen</t>
+  </si>
+  <si>
+    <t>Darstellung für neu spezifiziertes Spiel. Painter-Objekt.</t>
+  </si>
+  <si>
+    <t>Darstellung neues Spiel inkl. Schnittstellenkonzept</t>
   </si>
 </sst>
 </file>
@@ -282,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -324,6 +330,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -969,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,7 +1094,9 @@
       <c r="D7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E7"/>
+      <c r="E7" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -1100,43 +1111,35 @@
       <c r="D8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E8"/>
+      <c r="E8" s="15" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>2</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E9"/>
     </row>
     <row r="10" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <v>2</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
+      <c r="A10" s="7"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="13"/>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>28</v>
@@ -1147,15 +1150,21 @@
       <c r="D11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
+      <c r="E11"/>
     </row>
     <row r="12" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="13"/>
+      <c r="A12" s="7">
+        <v>2</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>

</xml_diff>